<commit_message>
map photo filepath update
</commit_message>
<xml_diff>
--- a/data/national_parks.xlsx
+++ b/data/national_parks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexreed/Documents/MEDS/Website/reedalexandria.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3401CA4-D3FF-714B-8F99-4B2800D2DF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E7899D-C65A-4344-93C0-C177BE0DBA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4760" yWindow="1680" windowWidth="23500" windowHeight="16780" xr2:uid="{64331E9F-51AE-FD44-8550-03B1AAF5833B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="186">
   <si>
     <t>Latitude</t>
   </si>
@@ -564,13 +565,43 @@
   </si>
   <si>
     <t>/Users/alexreed/Documents/MEDS/Website/reedalexandria.github.io/image/parks/zion.JPG</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/arches.jpeg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/bryce.JPG</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/glacier.jpeg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/teton.jpeg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/volcano.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/kings.jpeg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/rainier.JPG</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/sequoia.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/yosemite.JPG</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/reedalexandria/reedalexandria.github.io/main/image/parks/zion.JPG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -583,6 +614,14 @@
       <color rgb="FF3A3A3A"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -602,15 +641,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -926,7 +968,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,6 +1075,1500 @@
       <c r="G4" s="1" t="s">
         <v>165</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43.75</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-102.5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2">
+        <v>28804</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>29.25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-103.25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2">
+        <v>16235</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>25.65</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-80.08</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2">
+        <v>29400</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>38.57</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-107.72</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2">
+        <v>36454</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>37.57</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-112.18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2">
+        <v>10283</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-109.93</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2">
+        <v>23632</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-111.17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2">
+        <v>26285</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>32.17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-104.44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2">
+        <v>11092</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>34.01</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-119.42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="2">
+        <v>29285</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>33.78</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-80.78</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2">
+        <v>37935</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>42.94</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-122.1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="2">
+        <v>873</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>41.24</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-81.55</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="2">
+        <v>36810</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>36.24</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-116.82</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="2">
+        <v>34638</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>63.33</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-150.5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="2">
+        <v>6267</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>24.63</v>
+      </c>
+      <c r="B19" s="1">
+        <v>-82.87</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="2">
+        <v>33903</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>25.32</v>
+      </c>
+      <c r="B20" s="1">
+        <v>-80.930000000000007</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="2">
+        <v>12569</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>67.78</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-153.30000000000001</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="2">
+        <v>29557</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>38.630000000000003</v>
+      </c>
+      <c r="B22" s="1">
+        <v>-90.19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="2">
+        <v>43153</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>58.5</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-137</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="2">
+        <v>29557</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>48.8</v>
+      </c>
+      <c r="B24" s="1">
+        <v>-114</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3784</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>36.06</v>
+      </c>
+      <c r="B25" s="1">
+        <v>-112.14</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="2">
+        <v>6997</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43.73</v>
+      </c>
+      <c r="B26" s="1">
+        <v>-110.8</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="2">
+        <v>10650</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>38.979999999999997</v>
+      </c>
+      <c r="B27" s="1">
+        <v>-114.3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="2">
+        <v>31712</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="B28" s="1">
+        <v>-105.51</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="2">
+        <v>38243</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>35.68</v>
+      </c>
+      <c r="B29" s="1">
+        <v>-83.53</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="2">
+        <v>12585</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>31.92</v>
+      </c>
+      <c r="B30" s="1">
+        <v>-104.87</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="2">
+        <v>24395</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>20.72</v>
+      </c>
+      <c r="B31" s="1">
+        <v>-156.16999999999999</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="2">
+        <v>6058</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>19.38</v>
+      </c>
+      <c r="B32" s="1">
+        <v>-155.19999999999999</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="2">
+        <v>6058</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>34.51</v>
+      </c>
+      <c r="B33" s="1">
+        <v>-93.05</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="2">
+        <v>7734</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>41.653300000000002</v>
+      </c>
+      <c r="B34" s="1">
+        <v>-87.052400000000006</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="2">
+        <v>43511</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>48.1</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-88.55</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="2">
+        <v>14704</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>33.79</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-115.9</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="2">
+        <v>34638</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>58.5</v>
+      </c>
+      <c r="B37" s="1">
+        <v>-155</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="2">
+        <v>29557</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>59.92</v>
+      </c>
+      <c r="B38" s="1">
+        <v>-149.65</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="2">
+        <v>29557</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="B39" s="1">
+        <v>-118.55</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="2">
+        <v>14674</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>67.55</v>
+      </c>
+      <c r="B40" s="1">
+        <v>-159.28</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="2">
+        <v>29557</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>60.97</v>
+      </c>
+      <c r="B41" s="1">
+        <v>-153.41999999999999</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="2">
+        <v>29557</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>40.49</v>
+      </c>
+      <c r="B42" s="1">
+        <v>-121.51</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="2">
+        <v>6066</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>37.18</v>
+      </c>
+      <c r="B43" s="1">
+        <v>-86.1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="2">
+        <v>15158</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>37.18</v>
+      </c>
+      <c r="B44" s="1">
+        <v>-108.49</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2372</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>46.85</v>
+      </c>
+      <c r="B45" s="1">
+        <v>-121.75</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>48.7</v>
+      </c>
+      <c r="B46" s="1">
+        <v>-121.2</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="2">
+        <v>25113</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>47.97</v>
+      </c>
+      <c r="B47" s="1">
+        <v>-123.5</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E47" s="2">
+        <v>14060</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>35.07</v>
+      </c>
+      <c r="B48" s="1">
+        <v>-109.78</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="2">
+        <v>22989</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>36.479999999999997</v>
+      </c>
+      <c r="B49" s="1">
+        <v>-121.16</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="2">
+        <v>41284</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>41.3</v>
+      </c>
+      <c r="B50" s="1">
+        <v>-124</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="2">
+        <v>25113</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>40.4</v>
+      </c>
+      <c r="B51" s="1">
+        <v>-105.58</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="2">
+        <v>5505</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>32.25</v>
+      </c>
+      <c r="B52" s="1">
+        <v>-110.5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="2">
+        <v>34621</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>36.43</v>
+      </c>
+      <c r="B53" s="1">
+        <v>-118.68</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>38.53</v>
+      </c>
+      <c r="B54" s="1">
+        <v>-78.349999999999994</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E54" s="2">
+        <v>13144</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>46.97</v>
+      </c>
+      <c r="B55" s="1">
+        <v>-103.45</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E55" s="2">
+        <v>28804</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="B56" s="1">
+        <v>-64.73</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56" s="2">
+        <v>20669</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>48.5</v>
+      </c>
+      <c r="B57" s="1">
+        <v>-92.88</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E57" s="2">
+        <v>25941</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>43.57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>-103.48</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1105</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>61</v>
+      </c>
+      <c r="B59" s="1">
+        <v>-142</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E59" s="2">
+        <v>29557</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>44.6</v>
+      </c>
+      <c r="B60" s="1">
+        <v>-110.5</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>37.83</v>
+      </c>
+      <c r="B61" s="1">
+        <v>-119.5</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="B62" s="1">
+        <v>-113.05</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="2">
+        <v>7263</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{65707EF6-86CF-9946-BA2F-23DA681174CA}"/>
+    <hyperlink ref="H9" r:id="rId2" xr:uid="{2EA3BB03-1FCC-E14E-9F81-842E4D519091}"/>
+    <hyperlink ref="H24" r:id="rId3" xr:uid="{9DE07AC1-1BE8-4E4B-A216-A449E273EB6E}"/>
+    <hyperlink ref="H26" r:id="rId4" xr:uid="{1CF5645B-55EC-4C43-AF44-69A550513711}"/>
+    <hyperlink ref="H32" r:id="rId5" xr:uid="{B530D985-C00C-F24F-B946-AAD646D71AFA}"/>
+    <hyperlink ref="H39" r:id="rId6" xr:uid="{1B3A7668-AE95-F24B-8A96-0D7DDFC066C8}"/>
+    <hyperlink ref="H45" r:id="rId7" xr:uid="{0B32950D-288B-0A49-847D-D55AB65C3A30}"/>
+    <hyperlink ref="H53" r:id="rId8" xr:uid="{60D73EB8-258D-CC41-8AEB-E263DD6CCAC4}"/>
+    <hyperlink ref="H61" r:id="rId9" xr:uid="{5CC63DC3-9546-264A-AB62-59D8AEDB2030}"/>
+    <hyperlink ref="H62" r:id="rId10" xr:uid="{E8C3857F-0867-E94B-8C57-15260B96433C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748A87B3-63A8-3448-8F9A-64E4BE95B096}">
+  <dimension ref="A1:H62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44.35</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-68.209999999999994</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>6997</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>-14.25</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-170.68</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
+        <v>32447</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>38.68</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-109.57</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2">
+        <v>26249</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="H4" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
map photo filepath update2
</commit_message>
<xml_diff>
--- a/data/national_parks.xlsx
+++ b/data/national_parks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexreed/Documents/MEDS/Website/reedalexandria.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E7899D-C65A-4344-93C0-C177BE0DBA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF108F4-3FD2-2C4E-BAF8-A654AF6A1025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4760" yWindow="1680" windowWidth="23500" windowHeight="16780" xr2:uid="{64331E9F-51AE-FD44-8550-03B1AAF5833B}"/>
   </bookViews>
@@ -968,7 +968,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>